<commit_message>
add PMBus isolation resistors
</commit_message>
<xml_diff>
--- a/Manufacturing Files/bitaxeHex-302-BOM.xlsx
+++ b/Manufacturing Files/bitaxeHex-302-BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\bitaxeHex\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\bitaxeHex\Manufacturing Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{F67F2ECB-E90F-4465-A1A3-98E8B5BEDC74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC8472B-499E-455E-B3B6-3A2405EA9685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29220" yWindow="525" windowWidth="24165" windowHeight="14940"/>
+    <workbookView xWindow="29760" yWindow="240" windowWidth="24165" windowHeight="14940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bitaxeHex" sheetId="1" r:id="rId1"/>
@@ -655,9 +655,6 @@
     <t>RT0402BRD072KL</t>
   </si>
   <si>
-    <t>R42, R53, R73</t>
-  </si>
-  <si>
     <t>311-0.0JRCT-ND</t>
   </si>
   <si>
@@ -875,12 +872,15 @@
   </si>
   <si>
     <t>USB_C_Receptacle</t>
+  </si>
+  <si>
+    <t>R42, R53, R73, R109, R110, R111</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1740,11 +1740,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:J69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1759,7 +1759,7 @@
   <sheetData>
     <row r="1" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
@@ -2239,10 +2239,10 @@
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>211</v>
+        <v>284</v>
       </c>
       <c r="D27" s="4">
         <v>0</v>
@@ -2251,10 +2251,10 @@
         <v>124</v>
       </c>
       <c r="F27" t="s">
+        <v>211</v>
+      </c>
+      <c r="G27" s="3" t="s">
         <v>212</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
@@ -2554,7 +2554,7 @@
         <v>65</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
@@ -2614,7 +2614,7 @@
         <v>77</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
@@ -2722,19 +2722,19 @@
         <v>1</v>
       </c>
       <c r="C51" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="D51" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="E51" t="s">
         <v>220</v>
       </c>
-      <c r="E51" t="s">
+      <c r="F51" t="s">
         <v>221</v>
       </c>
-      <c r="F51" t="s">
+      <c r="G51" s="3" t="s">
         <v>222</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.25">
@@ -2742,19 +2742,19 @@
         <v>1</v>
       </c>
       <c r="C52" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="D52" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="E52" t="s">
         <v>225</v>
       </c>
-      <c r="E52" t="s">
+      <c r="F52" t="s">
         <v>226</v>
       </c>
-      <c r="F52" t="s">
-        <v>227</v>
-      </c>
       <c r="G52" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.25">
@@ -2762,19 +2762,19 @@
         <v>1</v>
       </c>
       <c r="C53" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="D53" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="D53" s="4" t="s">
+      <c r="E53" t="s">
         <v>229</v>
       </c>
-      <c r="E53" t="s">
+      <c r="F53" t="s">
         <v>230</v>
       </c>
-      <c r="F53" t="s">
-        <v>231</v>
-      </c>
       <c r="G53" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
@@ -2782,19 +2782,19 @@
         <v>1</v>
       </c>
       <c r="C54" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="D54" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="D54" s="4" t="s">
+      <c r="E54" t="s">
         <v>233</v>
       </c>
-      <c r="E54" t="s">
+      <c r="F54" t="s">
         <v>234</v>
       </c>
-      <c r="F54" t="s">
+      <c r="G54" s="3" t="s">
         <v>235</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.25">
@@ -2802,19 +2802,19 @@
         <v>1</v>
       </c>
       <c r="C55" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D55" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="D55" s="4" t="s">
+      <c r="E55" t="s">
         <v>238</v>
       </c>
-      <c r="E55" t="s">
+      <c r="F55" t="s">
         <v>239</v>
       </c>
-      <c r="F55" t="s">
+      <c r="G55" s="3" t="s">
         <v>240</v>
-      </c>
-      <c r="G55" s="3" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.25">
@@ -2822,19 +2822,19 @@
         <v>1</v>
       </c>
       <c r="C56" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="D56" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="D56" s="4" t="s">
+      <c r="E56" t="s">
         <v>243</v>
       </c>
-      <c r="E56" t="s">
+      <c r="F56" t="s">
         <v>244</v>
       </c>
-      <c r="F56" t="s">
+      <c r="G56" s="3" t="s">
         <v>245</v>
-      </c>
-      <c r="G56" s="3" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.25">
@@ -2842,19 +2842,19 @@
         <v>2</v>
       </c>
       <c r="C57" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="D57" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="D57" s="4" t="s">
+      <c r="E57" t="s">
         <v>248</v>
       </c>
-      <c r="E57" t="s">
+      <c r="F57" t="s">
         <v>249</v>
       </c>
-      <c r="F57" t="s">
+      <c r="G57" s="3" t="s">
         <v>250</v>
-      </c>
-      <c r="G57" s="3" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.25">
@@ -2862,19 +2862,19 @@
         <v>1</v>
       </c>
       <c r="C58" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="D58" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="D58" s="4" t="s">
+      <c r="E58" t="s">
         <v>253</v>
       </c>
-      <c r="E58" t="s">
+      <c r="F58" t="s">
         <v>254</v>
       </c>
-      <c r="F58" t="s">
+      <c r="G58" s="3" t="s">
         <v>255</v>
-      </c>
-      <c r="G58" s="3" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.25">
@@ -2882,19 +2882,19 @@
         <v>6</v>
       </c>
       <c r="C59" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="D59" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="E59" t="s">
         <v>258</v>
       </c>
-      <c r="E59" t="s">
+      <c r="F59" t="s">
         <v>259</v>
       </c>
-      <c r="F59" t="s">
+      <c r="G59" s="3" t="s">
         <v>260</v>
-      </c>
-      <c r="G59" s="3" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="60" spans="2:10" x14ac:dyDescent="0.25">
@@ -2902,13 +2902,13 @@
         <v>6</v>
       </c>
       <c r="C60" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="D60" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="D60" s="4" t="s">
-        <v>282</v>
-      </c>
       <c r="E60" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J60" s="3"/>
     </row>
@@ -2917,19 +2917,19 @@
         <v>3</v>
       </c>
       <c r="C61" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="D61" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="D61" s="4" t="s">
+      <c r="E61" t="s">
         <v>264</v>
       </c>
-      <c r="E61" t="s">
+      <c r="F61" t="s">
         <v>265</v>
       </c>
-      <c r="F61" t="s">
+      <c r="G61" s="3" t="s">
         <v>266</v>
-      </c>
-      <c r="G61" s="3" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.25">
@@ -2937,19 +2937,19 @@
         <v>2</v>
       </c>
       <c r="C62" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="D62" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="D62" s="4" t="s">
+      <c r="E62" t="s">
         <v>269</v>
       </c>
-      <c r="E62" t="s">
+      <c r="F62" t="s">
         <v>270</v>
       </c>
-      <c r="F62" t="s">
+      <c r="G62" s="3" t="s">
         <v>271</v>
-      </c>
-      <c r="G62" s="3" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="63" spans="2:10" x14ac:dyDescent="0.25">
@@ -2957,19 +2957,19 @@
         <v>1</v>
       </c>
       <c r="C63" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="D63" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="D63" s="4" t="s">
+      <c r="E63" t="s">
         <v>274</v>
       </c>
-      <c r="E63" t="s">
+      <c r="F63" t="s">
         <v>275</v>
       </c>
-      <c r="F63" t="s">
+      <c r="G63" s="3" t="s">
         <v>276</v>
-      </c>
-      <c r="G63" s="3" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="64" spans="2:10" x14ac:dyDescent="0.25">
@@ -2977,19 +2977,19 @@
         <v>2</v>
       </c>
       <c r="C64" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="D64" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="D64" s="4" t="s">
+      <c r="E64" t="s">
         <v>215</v>
       </c>
-      <c r="E64" t="s">
+      <c r="F64" t="s">
         <v>216</v>
       </c>
-      <c r="F64" t="s">
+      <c r="G64" s="3" t="s">
         <v>217</v>
-      </c>
-      <c r="G64" s="3" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.25">
@@ -3020,7 +3020,7 @@
         <v>93</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E66" t="s">
         <v>94</v>
@@ -3055,7 +3055,7 @@
         <v>100</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E68" t="s">
         <v>101</v>

</xml_diff>

<commit_message>
Set I2C address by choosing ADRSEL resistors
</commit_message>
<xml_diff>
--- a/Manufacturing Files/bitaxeHex-302-BOM.xlsx
+++ b/Manufacturing Files/bitaxeHex-302-BOM.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\bitaxeHex\Manufacturing Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC8472B-499E-455E-B3B6-3A2405EA9685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF40100-97DF-4F70-8D28-AE132F651BBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29760" yWindow="240" windowWidth="24165" windowHeight="14940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2235" yWindow="285" windowWidth="24165" windowHeight="14940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bitaxeHex" sheetId="1" r:id="rId1"/>
+    <sheet name="Config" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="310">
   <si>
     <t>Qty</t>
   </si>
@@ -388,9 +389,6 @@
     <t>2N7002KW</t>
   </si>
   <si>
-    <t>R1, R3, R5</t>
-  </si>
-  <si>
     <t>??</t>
   </si>
   <si>
@@ -433,9 +431,6 @@
     <t>RC0402FR-074K64L</t>
   </si>
   <si>
-    <t>R7, R15, R18, R22, R30, R47, R48, R59, R60, R67, R68, R75, R76, R81, R82, R86, R87, R100, R101, R105, R106</t>
-  </si>
-  <si>
     <t>10k</t>
   </si>
   <si>
@@ -875,6 +870,87 @@
   </si>
   <si>
     <t>R42, R53, R73, R109, R110, R111</t>
+  </si>
+  <si>
+    <t>Config resistors</t>
+  </si>
+  <si>
+    <t>Rvselt</t>
+  </si>
+  <si>
+    <t>Radrt</t>
+  </si>
+  <si>
+    <t>Rvselb</t>
+  </si>
+  <si>
+    <t>Rmsel1t</t>
+  </si>
+  <si>
+    <t>Radrb</t>
+  </si>
+  <si>
+    <t>Rmsel1b</t>
+  </si>
+  <si>
+    <t>MSEL2</t>
+  </si>
+  <si>
+    <t>VSEL</t>
+  </si>
+  <si>
+    <t>ADRSEL</t>
+  </si>
+  <si>
+    <t>MSEL1</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Rvalue</t>
+  </si>
+  <si>
+    <t>top</t>
+  </si>
+  <si>
+    <t>bottom</t>
+  </si>
+  <si>
+    <t>0R</t>
+  </si>
+  <si>
+    <t>R3, R7, R15, R18, R22, R30, R47, R48, R59, R60, R67, R68, R75, R76, R81, R82, R86, R87, R100, R101, R105, R106</t>
+  </si>
+  <si>
+    <t>R1, R5</t>
+  </si>
+  <si>
+    <t>RefDes</t>
+  </si>
+  <si>
+    <t>Pin</t>
+  </si>
+  <si>
+    <t>Rmsel2t</t>
+  </si>
+  <si>
+    <t>Rmsel2b</t>
+  </si>
+  <si>
+    <t>205.0K</t>
   </si>
 </sst>
 </file>
@@ -1375,7 +1451,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1385,6 +1461,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1743,8 +1824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:J69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1759,7 +1840,7 @@
   <sheetData>
     <row r="1" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
@@ -1784,16 +1865,16 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" t="s">
         <v>123</v>
-      </c>
-      <c r="E4" t="s">
-        <v>124</v>
       </c>
       <c r="G4" s="3"/>
     </row>
@@ -1802,19 +1883,19 @@
         <v>1</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" t="s">
+        <v>123</v>
+      </c>
+      <c r="F5" t="s">
         <v>126</v>
       </c>
-      <c r="E5" t="s">
-        <v>124</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="G5" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
@@ -1822,19 +1903,19 @@
         <v>1</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" t="s">
+        <v>123</v>
+      </c>
+      <c r="F6" t="s">
         <v>130</v>
       </c>
-      <c r="E6" t="s">
-        <v>124</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="G6" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
@@ -1842,39 +1923,39 @@
         <v>1</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F7" t="s">
         <v>134</v>
       </c>
-      <c r="E7" t="s">
-        <v>124</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="G7" s="3" t="s">
         <v>135</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E8" t="s">
+        <v>123</v>
+      </c>
+      <c r="F8" t="s">
         <v>137</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="E8" t="s">
-        <v>124</v>
-      </c>
-      <c r="F8" t="s">
-        <v>139</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -1882,19 +1963,19 @@
         <v>1</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="E9" t="s">
+        <v>123</v>
+      </c>
+      <c r="F9" t="s">
         <v>141</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="G9" s="3" t="s">
         <v>142</v>
-      </c>
-      <c r="E9" t="s">
-        <v>124</v>
-      </c>
-      <c r="F9" t="s">
-        <v>143</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -1902,19 +1983,19 @@
         <v>2</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="E10" t="s">
+        <v>123</v>
+      </c>
+      <c r="F10" t="s">
         <v>145</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="G10" s="3" t="s">
         <v>146</v>
-      </c>
-      <c r="E10" t="s">
-        <v>124</v>
-      </c>
-      <c r="F10" t="s">
-        <v>147</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
@@ -1922,19 +2003,19 @@
         <v>1</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="E11" t="s">
+        <v>123</v>
+      </c>
+      <c r="F11" t="s">
         <v>149</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="G11" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="E11" t="s">
-        <v>124</v>
-      </c>
-      <c r="F11" t="s">
-        <v>151</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1942,19 +2023,19 @@
         <v>10</v>
       </c>
       <c r="C12" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E12" t="s">
+        <v>123</v>
+      </c>
+      <c r="F12" t="s">
         <v>153</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="G12" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="E12" t="s">
-        <v>124</v>
-      </c>
-      <c r="F12" t="s">
-        <v>155</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
@@ -1962,19 +2043,19 @@
         <v>2</v>
       </c>
       <c r="C13" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="E13" t="s">
+        <v>123</v>
+      </c>
+      <c r="F13" t="s">
         <v>157</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="G13" s="3" t="s">
         <v>158</v>
-      </c>
-      <c r="E13" t="s">
-        <v>124</v>
-      </c>
-      <c r="F13" t="s">
-        <v>159</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
@@ -1982,19 +2063,19 @@
         <v>1</v>
       </c>
       <c r="C14" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E14" t="s">
+        <v>123</v>
+      </c>
+      <c r="F14" t="s">
         <v>161</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="G14" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="E14" t="s">
-        <v>124</v>
-      </c>
-      <c r="F14" t="s">
-        <v>163</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
@@ -2002,19 +2083,19 @@
         <v>1</v>
       </c>
       <c r="C15" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="E15" t="s">
         <v>165</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="F15" t="s">
         <v>166</v>
       </c>
-      <c r="E15" t="s">
+      <c r="G15" s="3" t="s">
         <v>167</v>
-      </c>
-      <c r="F15" t="s">
-        <v>168</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
@@ -2022,19 +2103,19 @@
         <v>1</v>
       </c>
       <c r="C16" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="E16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F16" t="s">
         <v>170</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="G16" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="E16" t="s">
-        <v>124</v>
-      </c>
-      <c r="F16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -2042,19 +2123,19 @@
         <v>1</v>
       </c>
       <c r="C17" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="E17" t="s">
+        <v>123</v>
+      </c>
+      <c r="F17" t="s">
         <v>174</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="G17" s="3" t="s">
         <v>175</v>
-      </c>
-      <c r="E17" t="s">
-        <v>124</v>
-      </c>
-      <c r="F17" t="s">
-        <v>176</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
@@ -2062,19 +2143,19 @@
         <v>1</v>
       </c>
       <c r="C18" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="E18" t="s">
+        <v>123</v>
+      </c>
+      <c r="F18" t="s">
         <v>178</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="G18" s="3" t="s">
         <v>179</v>
-      </c>
-      <c r="E18" t="s">
-        <v>124</v>
-      </c>
-      <c r="F18" t="s">
-        <v>180</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2082,19 +2163,19 @@
         <v>19</v>
       </c>
       <c r="C19" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="E19" t="s">
+        <v>123</v>
+      </c>
+      <c r="F19" t="s">
         <v>182</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="G19" s="3" t="s">
         <v>183</v>
-      </c>
-      <c r="E19" t="s">
-        <v>124</v>
-      </c>
-      <c r="F19" t="s">
-        <v>184</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
@@ -2102,19 +2183,19 @@
         <v>2</v>
       </c>
       <c r="C20" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="E20" t="s">
+        <v>123</v>
+      </c>
+      <c r="F20" t="s">
         <v>186</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="G20" s="3" t="s">
         <v>187</v>
-      </c>
-      <c r="E20" t="s">
-        <v>124</v>
-      </c>
-      <c r="F20" t="s">
-        <v>188</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
@@ -2122,19 +2203,19 @@
         <v>2</v>
       </c>
       <c r="C21" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="E21" t="s">
+        <v>123</v>
+      </c>
+      <c r="F21" t="s">
         <v>190</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="G21" s="3" t="s">
         <v>191</v>
-      </c>
-      <c r="E21" t="s">
-        <v>124</v>
-      </c>
-      <c r="F21" t="s">
-        <v>192</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
@@ -2142,19 +2223,19 @@
         <v>2</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F22" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
@@ -2162,19 +2243,19 @@
         <v>3</v>
       </c>
       <c r="C23" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="E23" t="s">
+        <v>123</v>
+      </c>
+      <c r="F23" t="s">
         <v>196</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="G23" s="3" t="s">
         <v>197</v>
-      </c>
-      <c r="E23" t="s">
-        <v>124</v>
-      </c>
-      <c r="F23" t="s">
-        <v>198</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2182,19 +2263,19 @@
         <v>20</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D24" s="4">
         <v>33</v>
       </c>
       <c r="E24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F24" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
@@ -2202,19 +2283,19 @@
         <v>6</v>
       </c>
       <c r="C25" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="D25" s="4">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>202</v>
+      </c>
+      <c r="F25" t="s">
         <v>203</v>
       </c>
-      <c r="D25" s="4">
-        <v>1</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="G25" s="3" t="s">
         <v>204</v>
-      </c>
-      <c r="F25" t="s">
-        <v>205</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
@@ -2222,19 +2303,19 @@
         <v>3</v>
       </c>
       <c r="C26" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="E26" t="s">
+        <v>123</v>
+      </c>
+      <c r="F26" t="s">
         <v>207</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="G26" s="3" t="s">
         <v>208</v>
-      </c>
-      <c r="E26" t="s">
-        <v>124</v>
-      </c>
-      <c r="F26" t="s">
-        <v>209</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
@@ -2242,19 +2323,19 @@
         <v>6</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D27" s="4">
         <v>0</v>
       </c>
       <c r="E27" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F27" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
@@ -2554,7 +2635,7 @@
         <v>65</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
@@ -2614,7 +2695,7 @@
         <v>77</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
@@ -2722,19 +2803,19 @@
         <v>1</v>
       </c>
       <c r="C51" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="E51" t="s">
         <v>218</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="F51" t="s">
         <v>219</v>
       </c>
-      <c r="E51" t="s">
+      <c r="G51" s="3" t="s">
         <v>220</v>
-      </c>
-      <c r="F51" t="s">
-        <v>221</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.25">
@@ -2742,19 +2823,19 @@
         <v>1</v>
       </c>
       <c r="C52" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="E52" t="s">
         <v>223</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="F52" t="s">
         <v>224</v>
       </c>
-      <c r="E52" t="s">
-        <v>225</v>
-      </c>
-      <c r="F52" t="s">
-        <v>226</v>
-      </c>
       <c r="G52" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.25">
@@ -2762,19 +2843,19 @@
         <v>1</v>
       </c>
       <c r="C53" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="E53" t="s">
         <v>227</v>
       </c>
-      <c r="D53" s="4" t="s">
+      <c r="F53" t="s">
         <v>228</v>
       </c>
-      <c r="E53" t="s">
-        <v>229</v>
-      </c>
-      <c r="F53" t="s">
-        <v>230</v>
-      </c>
       <c r="G53" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
@@ -2782,19 +2863,19 @@
         <v>1</v>
       </c>
       <c r="C54" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E54" t="s">
         <v>231</v>
       </c>
-      <c r="D54" s="4" t="s">
+      <c r="F54" t="s">
         <v>232</v>
       </c>
-      <c r="E54" t="s">
+      <c r="G54" s="3" t="s">
         <v>233</v>
-      </c>
-      <c r="F54" t="s">
-        <v>234</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.25">
@@ -2802,19 +2883,19 @@
         <v>1</v>
       </c>
       <c r="C55" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="E55" t="s">
         <v>236</v>
       </c>
-      <c r="D55" s="4" t="s">
+      <c r="F55" t="s">
         <v>237</v>
       </c>
-      <c r="E55" t="s">
+      <c r="G55" s="3" t="s">
         <v>238</v>
-      </c>
-      <c r="F55" t="s">
-        <v>239</v>
-      </c>
-      <c r="G55" s="3" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.25">
@@ -2822,19 +2903,19 @@
         <v>1</v>
       </c>
       <c r="C56" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="E56" t="s">
         <v>241</v>
       </c>
-      <c r="D56" s="4" t="s">
+      <c r="F56" t="s">
         <v>242</v>
       </c>
-      <c r="E56" t="s">
+      <c r="G56" s="3" t="s">
         <v>243</v>
-      </c>
-      <c r="F56" t="s">
-        <v>244</v>
-      </c>
-      <c r="G56" s="3" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.25">
@@ -2842,19 +2923,19 @@
         <v>2</v>
       </c>
       <c r="C57" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="E57" t="s">
         <v>246</v>
       </c>
-      <c r="D57" s="4" t="s">
+      <c r="F57" t="s">
         <v>247</v>
       </c>
-      <c r="E57" t="s">
+      <c r="G57" s="3" t="s">
         <v>248</v>
-      </c>
-      <c r="F57" t="s">
-        <v>249</v>
-      </c>
-      <c r="G57" s="3" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.25">
@@ -2862,19 +2943,19 @@
         <v>1</v>
       </c>
       <c r="C58" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="E58" t="s">
         <v>251</v>
       </c>
-      <c r="D58" s="4" t="s">
+      <c r="F58" t="s">
         <v>252</v>
       </c>
-      <c r="E58" t="s">
+      <c r="G58" s="3" t="s">
         <v>253</v>
-      </c>
-      <c r="F58" t="s">
-        <v>254</v>
-      </c>
-      <c r="G58" s="3" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.25">
@@ -2882,19 +2963,19 @@
         <v>6</v>
       </c>
       <c r="C59" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="E59" t="s">
         <v>256</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="F59" t="s">
         <v>257</v>
       </c>
-      <c r="E59" t="s">
+      <c r="G59" s="3" t="s">
         <v>258</v>
-      </c>
-      <c r="F59" t="s">
-        <v>259</v>
-      </c>
-      <c r="G59" s="3" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="60" spans="2:10" x14ac:dyDescent="0.25">
@@ -2902,13 +2983,13 @@
         <v>6</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E60" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="J60" s="3"/>
     </row>
@@ -2917,19 +2998,19 @@
         <v>3</v>
       </c>
       <c r="C61" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="E61" t="s">
         <v>262</v>
       </c>
-      <c r="D61" s="4" t="s">
+      <c r="F61" t="s">
         <v>263</v>
       </c>
-      <c r="E61" t="s">
+      <c r="G61" s="3" t="s">
         <v>264</v>
-      </c>
-      <c r="F61" t="s">
-        <v>265</v>
-      </c>
-      <c r="G61" s="3" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.25">
@@ -2937,19 +3018,19 @@
         <v>2</v>
       </c>
       <c r="C62" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="E62" t="s">
         <v>267</v>
       </c>
-      <c r="D62" s="4" t="s">
+      <c r="F62" t="s">
         <v>268</v>
       </c>
-      <c r="E62" t="s">
+      <c r="G62" s="3" t="s">
         <v>269</v>
-      </c>
-      <c r="F62" t="s">
-        <v>270</v>
-      </c>
-      <c r="G62" s="3" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="63" spans="2:10" x14ac:dyDescent="0.25">
@@ -2957,19 +3038,19 @@
         <v>1</v>
       </c>
       <c r="C63" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="E63" t="s">
         <v>272</v>
       </c>
-      <c r="D63" s="4" t="s">
+      <c r="F63" t="s">
         <v>273</v>
       </c>
-      <c r="E63" t="s">
+      <c r="G63" s="3" t="s">
         <v>274</v>
-      </c>
-      <c r="F63" t="s">
-        <v>275</v>
-      </c>
-      <c r="G63" s="3" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="64" spans="2:10" x14ac:dyDescent="0.25">
@@ -2977,19 +3058,19 @@
         <v>2</v>
       </c>
       <c r="C64" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="E64" t="s">
         <v>213</v>
       </c>
-      <c r="D64" s="4" t="s">
+      <c r="F64" t="s">
         <v>214</v>
       </c>
-      <c r="E64" t="s">
+      <c r="G64" s="3" t="s">
         <v>215</v>
-      </c>
-      <c r="F64" t="s">
-        <v>216</v>
-      </c>
-      <c r="G64" s="3" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.25">
@@ -3020,7 +3101,7 @@
         <v>93</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E66" t="s">
         <v>94</v>
@@ -3055,7 +3136,7 @@
         <v>100</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E68" t="s">
         <v>101</v>
@@ -3085,6 +3166,195 @@
       </c>
       <c r="G69" s="3">
         <v>470531000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7076F42F-395B-4B2A-80FC-BC7D4FBCDC22}">
+  <dimension ref="B1:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="7.85546875" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="C4" t="s">
+        <v>307</v>
+      </c>
+      <c r="D4" t="s">
+        <v>300</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="6"/>
+      <c r="C5" t="s">
+        <v>308</v>
+      </c>
+      <c r="D5" t="s">
+        <v>301</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="C6" t="s">
+        <v>284</v>
+      </c>
+      <c r="D6" t="s">
+        <v>300</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="F6" s="8">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="6"/>
+      <c r="C7" t="s">
+        <v>286</v>
+      </c>
+      <c r="D7" t="s">
+        <v>301</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="C8" t="s">
+        <v>285</v>
+      </c>
+      <c r="D8" t="s">
+        <v>300</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="F8" s="8">
+        <v>6</v>
+      </c>
+      <c r="G8" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="6"/>
+      <c r="C9" t="s">
+        <v>288</v>
+      </c>
+      <c r="D9" t="s">
+        <v>301</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="F9" s="8">
+        <v>4</v>
+      </c>
+      <c r="G9" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="C10" t="s">
+        <v>287</v>
+      </c>
+      <c r="D10" t="s">
+        <v>300</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="F10" s="8">
+        <v>2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="6"/>
+      <c r="C11" t="s">
+        <v>289</v>
+      </c>
+      <c r="D11" t="s">
+        <v>301</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="F11" s="8">
+        <v>15</v>
+      </c>
+      <c r="G11" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BOM adjustments to R28, R29, config resistors
</commit_message>
<xml_diff>
--- a/Manufacturing Files/bitaxeHex-302-BOM.xlsx
+++ b/Manufacturing Files/bitaxeHex-302-BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\bitaxeHex\Manufacturing Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF40100-97DF-4F70-8D28-AE132F651BBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0633C286-6562-43A6-B10C-F6E93265E8CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2235" yWindow="285" windowWidth="24165" windowHeight="14940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="465" windowWidth="25485" windowHeight="14940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bitaxeHex" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="309">
   <si>
     <t>Qty</t>
   </si>
@@ -599,9 +599,6 @@
     <t>RC0402FR-135K6L</t>
   </si>
   <si>
-    <t>R28, R29</t>
-  </si>
-  <si>
     <t>10K</t>
   </si>
   <si>
@@ -932,9 +929,6 @@
     <t>0R</t>
   </si>
   <si>
-    <t>R3, R7, R15, R18, R22, R30, R47, R48, R59, R60, R67, R68, R75, R76, R81, R82, R86, R87, R100, R101, R105, R106</t>
-  </si>
-  <si>
     <t>R1, R5</t>
   </si>
   <si>
@@ -951,6 +945,9 @@
   </si>
   <si>
     <t>205.0K</t>
+  </si>
+  <si>
+    <t>R3, R7, R15, R18, R22, R28, R29, R30, R47, R48, R59, R60, R67, R68, R75, R76, R81, R82, R86, R87, R100, R101, R105, R106</t>
   </si>
 </sst>
 </file>
@@ -1822,10 +1819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:J69"/>
+  <dimension ref="B1:J68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1840,7 +1837,7 @@
   <sheetData>
     <row r="1" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
@@ -1868,7 +1865,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>122</v>
@@ -1940,10 +1937,10 @@
     </row>
     <row r="8" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>136</v>
@@ -2220,202 +2217,202 @@
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E22" t="s">
         <v>123</v>
       </c>
       <c r="F22" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>195</v>
+        <v>197</v>
+      </c>
+      <c r="D23" s="4">
+        <v>33</v>
       </c>
       <c r="E23" t="s">
         <v>123</v>
       </c>
       <c r="F23" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D24" s="4">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>123</v>
+        <v>201</v>
       </c>
       <c r="F24" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="D25" s="4">
-        <v>1</v>
+        <v>204</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>205</v>
       </c>
       <c r="E25" t="s">
-        <v>202</v>
+        <v>123</v>
       </c>
       <c r="F25" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>206</v>
+        <v>281</v>
+      </c>
+      <c r="D26" s="4">
+        <v>0</v>
       </c>
       <c r="E26" t="s">
         <v>123</v>
       </c>
       <c r="F26" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="D27" s="4">
-        <v>0</v>
+      <c r="D27" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="E27" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
       <c r="F27" t="s">
-        <v>209</v>
+        <v>9</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>210</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E28" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F28" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E29" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F29" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E30" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F30" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E31" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F31" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
@@ -2423,99 +2420,99 @@
         <v>1</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E32" t="s">
         <v>28</v>
       </c>
       <c r="F32" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" ht="165" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33">
-        <v>1</v>
+        <v>99</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D33" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" t="s">
+        <v>36</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>27</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="E33" t="s">
-        <v>28</v>
-      </c>
-      <c r="F33" t="s">
-        <v>33</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" ht="165" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34">
-        <v>99</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="E34" t="s">
         <v>8</v>
       </c>
       <c r="F34" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="E35" t="s">
         <v>8</v>
       </c>
       <c r="F35" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="E36" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="F36" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
@@ -2523,39 +2520,39 @@
         <v>2</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="E37" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="F37" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E38" t="s">
         <v>8</v>
       </c>
       <c r="F38" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
@@ -2563,19 +2560,19 @@
         <v>1</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E39" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="F39" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
@@ -2583,19 +2580,19 @@
         <v>1</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="E40" t="s">
         <v>18</v>
       </c>
       <c r="F40" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
@@ -2603,39 +2600,39 @@
         <v>1</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="E41" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="F41" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>62</v>
+        <v>275</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E42" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="F42" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>276</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
@@ -2643,19 +2640,19 @@
         <v>2</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E43" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="F43" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
@@ -2663,59 +2660,59 @@
         <v>2</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E44" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="F44" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>73</v>
+        <v>276</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E45" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="F45" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>277</v>
+        <v>82</v>
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>79</v>
+        <v>109</v>
       </c>
       <c r="E46" t="s">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="F46" t="s">
-        <v>81</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>82</v>
+        <v>111</v>
+      </c>
+      <c r="G46" s="3">
+        <v>78438357082</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.25">
@@ -2723,19 +2720,19 @@
         <v>1</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E47" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F47" t="s">
-        <v>111</v>
-      </c>
-      <c r="G47" s="3">
-        <v>78438357082</v>
+        <v>115</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.25">
@@ -2743,19 +2740,19 @@
         <v>1</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E48" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="F48" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.25">
@@ -2763,19 +2760,19 @@
         <v>1</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="E49" t="s">
-        <v>119</v>
+        <v>85</v>
       </c>
       <c r="F49" t="s">
-        <v>120</v>
+        <v>86</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>121</v>
+        <v>87</v>
       </c>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
@@ -2783,19 +2780,19 @@
         <v>1</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>83</v>
+        <v>215</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>84</v>
+        <v>216</v>
       </c>
       <c r="E50" t="s">
-        <v>85</v>
+        <v>217</v>
       </c>
       <c r="F50" t="s">
-        <v>86</v>
+        <v>218</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>87</v>
+        <v>219</v>
       </c>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.25">
@@ -2803,19 +2800,19 @@
         <v>1</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="E51" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="F51" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.25">
@@ -2823,19 +2820,19 @@
         <v>1</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="E52" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="F52" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.25">
@@ -2843,19 +2840,19 @@
         <v>1</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="E53" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="F53" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
@@ -2863,19 +2860,19 @@
         <v>1</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="E54" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="F54" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.25">
@@ -2883,79 +2880,79 @@
         <v>1</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="E55" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="F55" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="E56" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="F56" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="E57" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="F57" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B58">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="E58" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="F58" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.25">
@@ -2963,94 +2960,94 @@
         <v>6</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>254</v>
+        <v>277</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>255</v>
+        <v>278</v>
       </c>
       <c r="E59" t="s">
-        <v>256</v>
-      </c>
-      <c r="F59" t="s">
-        <v>257</v>
-      </c>
-      <c r="G59" s="3" t="s">
         <v>258</v>
       </c>
+      <c r="J59" s="3"/>
     </row>
     <row r="60" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B60">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>278</v>
+        <v>259</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>279</v>
+        <v>260</v>
       </c>
       <c r="E60" t="s">
-        <v>259</v>
-      </c>
-      <c r="J60" s="3"/>
+        <v>261</v>
+      </c>
+      <c r="F60" t="s">
+        <v>262</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B61">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="E61" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="F61" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B62">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="E62" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="F62" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="63" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B63">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>270</v>
+        <v>210</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>271</v>
+        <v>211</v>
       </c>
       <c r="E63" t="s">
-        <v>272</v>
+        <v>212</v>
       </c>
       <c r="F63" t="s">
-        <v>273</v>
+        <v>213</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>274</v>
+        <v>214</v>
       </c>
     </row>
     <row r="64" spans="2:10" x14ac:dyDescent="0.25">
@@ -3058,113 +3055,93 @@
         <v>2</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>211</v>
+        <v>88</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>212</v>
+        <v>89</v>
       </c>
       <c r="E64" t="s">
-        <v>213</v>
+        <v>90</v>
       </c>
       <c r="F64" t="s">
-        <v>214</v>
+        <v>91</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>215</v>
+        <v>92</v>
       </c>
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B65">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>89</v>
+        <v>279</v>
       </c>
       <c r="E65" t="s">
-        <v>90</v>
-      </c>
-      <c r="F65" t="s">
-        <v>91</v>
-      </c>
-      <c r="G65" s="3" t="s">
-        <v>92</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="G65" s="3"/>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B66">
         <v>1</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>280</v>
+        <v>96</v>
       </c>
       <c r="E66" t="s">
-        <v>94</v>
-      </c>
-      <c r="G66" s="3"/>
+        <v>97</v>
+      </c>
+      <c r="F66" t="s">
+        <v>98</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B67">
         <v>1</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>96</v>
+        <v>280</v>
       </c>
       <c r="E67" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="F67" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B68">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>281</v>
+        <v>105</v>
       </c>
       <c r="E68" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="F68" t="s">
-        <v>102</v>
-      </c>
-      <c r="G68" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B69">
-        <v>2</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="E69" t="s">
-        <v>106</v>
-      </c>
-      <c r="F69" t="s">
         <v>107</v>
       </c>
-      <c r="G69" s="3">
+      <c r="G68" s="3">
         <v>470531000</v>
       </c>
     </row>
@@ -3190,7 +3167,7 @@
   <sheetData>
     <row r="1" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
@@ -3198,60 +3175,60 @@
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>298</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F4" s="8"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="6"/>
       <c r="C5" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>124</v>
@@ -3266,10 +3243,10 @@
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="6"/>
       <c r="C7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>132</v>
@@ -3283,51 +3260,51 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D8" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F8" s="8">
         <v>6</v>
       </c>
       <c r="G8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
       <c r="C9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F9" s="8">
         <v>4</v>
       </c>
       <c r="G9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D10" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>128</v>
@@ -3336,16 +3313,16 @@
         <v>2</v>
       </c>
       <c r="G10" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="C11" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D11" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>147</v>

</xml_diff>

<commit_message>
update to BOM for config resistors
</commit_message>
<xml_diff>
--- a/Manufacturing Files/bitaxeHex-302-BOM.xlsx
+++ b/Manufacturing Files/bitaxeHex-302-BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\bitaxeHex\Manufacturing Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0633C286-6562-43A6-B10C-F6E93265E8CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068CF9AD-24F5-461A-A318-F4A1ED55878A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="465" windowWidth="25485" windowHeight="14940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="25485" windowHeight="14940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bitaxeHex" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="311">
   <si>
     <t>Qty</t>
   </si>
@@ -389,9 +389,6 @@
     <t>2N7002KW</t>
   </si>
   <si>
-    <t>??</t>
-  </si>
-  <si>
     <t>Resistor_SMD:R_0402_1005Metric</t>
   </si>
   <si>
@@ -401,36 +398,15 @@
     <t>2.05K</t>
   </si>
   <si>
-    <t>YAG3096CT-ND</t>
-  </si>
-  <si>
-    <t>RC0402FR-072K05L</t>
-  </si>
-  <si>
     <t>R4</t>
   </si>
   <si>
-    <t>205K</t>
-  </si>
-  <si>
-    <t>YAG3050CT-ND</t>
-  </si>
-  <si>
-    <t>RC0402FR-07205KL</t>
-  </si>
-  <si>
     <t>R6</t>
   </si>
   <si>
     <t>4.64K</t>
   </si>
   <si>
-    <t>311-4.64KLRCT-ND</t>
-  </si>
-  <si>
-    <t>RC0402FR-074K64L</t>
-  </si>
-  <si>
     <t>10k</t>
   </si>
   <si>
@@ -470,12 +446,6 @@
     <t>82.5K</t>
   </si>
   <si>
-    <t>311-82.5KLRCT-ND</t>
-  </si>
-  <si>
-    <t>RC0402FR-0782K5L</t>
-  </si>
-  <si>
     <t>R11, R31, R32, R33, R54, R55, R57, R88, R89, R90</t>
   </si>
   <si>
@@ -929,9 +899,6 @@
     <t>0R</t>
   </si>
   <si>
-    <t>R1, R5</t>
-  </si>
-  <si>
     <t>RefDes</t>
   </si>
   <si>
@@ -947,7 +914,46 @@
     <t>205.0K</t>
   </si>
   <si>
-    <t>R3, R7, R15, R18, R22, R28, R29, R30, R47, R48, R59, R60, R67, R68, R75, R76, R81, R82, R86, R87, R100, R101, R105, R106</t>
+    <t>DNP</t>
+  </si>
+  <si>
+    <t>17.8K</t>
+  </si>
+  <si>
+    <t>RMCF0402FT17K8TR-ND</t>
+  </si>
+  <si>
+    <t>RMCF0402FT17K8TR</t>
+  </si>
+  <si>
+    <t>RMCF0402FT17K8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RMCF0402FT10K0TR-ND</t>
+  </si>
+  <si>
+    <t>RMCF0402FT10K0</t>
+  </si>
+  <si>
+    <t>31.6K</t>
+  </si>
+  <si>
+    <t>YAG3115TR-ND</t>
+  </si>
+  <si>
+    <t>RC0402FR-0731K6L</t>
+  </si>
+  <si>
+    <t>26.1K</t>
+  </si>
+  <si>
+    <t>311-26.1KLRTR-ND</t>
+  </si>
+  <si>
+    <t>RC0402FR-0726K1L</t>
+  </si>
+  <si>
+    <t>R15, R18, R22, R28, R29, R30, R47, R48, R59, R60, R67, R68, R75, R76, R81, R82, R86, R87, R100, R101, R105, R106</t>
   </si>
 </sst>
 </file>
@@ -1448,7 +1454,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1463,6 +1469,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1819,10 +1828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:J68"/>
+  <dimension ref="B1:J71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD22"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1837,7 +1846,7 @@
   <sheetData>
     <row r="1" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
@@ -1862,16 +1871,16 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="D4" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="E4" t="s">
         <v>122</v>
-      </c>
-      <c r="E4" t="s">
-        <v>123</v>
       </c>
       <c r="G4" s="3"/>
     </row>
@@ -1880,39 +1889,33 @@
         <v>1</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>125</v>
+        <v>298</v>
       </c>
       <c r="E5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F5" t="s">
-        <v>126</v>
+        <v>299</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>127</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>129</v>
+      <c r="C6" t="s">
+        <v>285</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>297</v>
       </c>
       <c r="E6" t="s">
-        <v>123</v>
-      </c>
-      <c r="F6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
@@ -1920,39 +1923,39 @@
         <v>1</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>133</v>
+        <v>298</v>
       </c>
       <c r="E7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F7" t="s">
-        <v>134</v>
+        <v>299</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>308</v>
+        <v>284</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>136</v>
+        <v>182</v>
       </c>
       <c r="E8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F8" t="s">
-        <v>137</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>138</v>
+        <v>302</v>
+      </c>
+      <c r="G8" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -1960,39 +1963,33 @@
         <v>1</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>140</v>
+        <v>304</v>
       </c>
       <c r="E9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F9" t="s">
-        <v>141</v>
+        <v>305</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>142</v>
+        <v>306</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>144</v>
+        <v>286</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>297</v>
       </c>
       <c r="E10" t="s">
-        <v>123</v>
-      </c>
-      <c r="F10" t="s">
-        <v>145</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
@@ -2000,119 +1997,119 @@
         <v>1</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>148</v>
+        <v>307</v>
       </c>
       <c r="E11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F11" t="s">
-        <v>149</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>308</v>
+      </c>
+      <c r="G11" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>151</v>
+        <v>310</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="E12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F12" t="s">
-        <v>153</v>
+        <v>129</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>154</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>155</v>
+        <v>131</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>156</v>
+        <v>132</v>
       </c>
       <c r="E13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F13" t="s">
-        <v>157</v>
+        <v>133</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>158</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="E14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F14" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>163</v>
+        <v>141</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>164</v>
+        <v>142</v>
       </c>
       <c r="E15" t="s">
-        <v>165</v>
+        <v>122</v>
       </c>
       <c r="F15" t="s">
-        <v>166</v>
+        <v>143</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>167</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>168</v>
+        <v>145</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="E16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F16" t="s">
-        <v>170</v>
+        <v>147</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>171</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -2120,19 +2117,19 @@
         <v>1</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>172</v>
+        <v>149</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="E17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F17" t="s">
-        <v>174</v>
+        <v>151</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>175</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
@@ -2140,139 +2137,139 @@
         <v>1</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>176</v>
+        <v>153</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>177</v>
+        <v>154</v>
       </c>
       <c r="E18" t="s">
-        <v>123</v>
+        <v>155</v>
       </c>
       <c r="F18" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>180</v>
+        <v>158</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>181</v>
+        <v>159</v>
       </c>
       <c r="E19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F19" t="s">
-        <v>182</v>
+        <v>160</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>183</v>
+        <v>161</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>184</v>
+        <v>162</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>185</v>
+        <v>163</v>
       </c>
       <c r="E20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F20" t="s">
-        <v>186</v>
+        <v>164</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>187</v>
+        <v>165</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="E21" t="s">
+        <v>122</v>
+      </c>
+      <c r="F21" t="s">
+        <v>168</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>19</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="E22" t="s">
+        <v>122</v>
+      </c>
+      <c r="F22" t="s">
+        <v>172</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23">
         <v>2</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="E21" t="s">
-        <v>123</v>
-      </c>
-      <c r="F21" t="s">
-        <v>190</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22">
-        <v>3</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="E22" t="s">
-        <v>123</v>
-      </c>
-      <c r="F22" t="s">
-        <v>195</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23">
-        <v>20</v>
-      </c>
       <c r="C23" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="D23" s="4">
-        <v>33</v>
+        <v>174</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>175</v>
       </c>
       <c r="E23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F23" t="s">
-        <v>198</v>
+        <v>176</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>199</v>
+        <v>177</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="D24" s="4">
-        <v>1</v>
+        <v>178</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>179</v>
       </c>
       <c r="E24" t="s">
-        <v>201</v>
+        <v>122</v>
       </c>
       <c r="F24" t="s">
-        <v>202</v>
+        <v>180</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>203</v>
+        <v>181</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
@@ -2280,199 +2277,199 @@
         <v>3</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="E25" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F25" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>281</v>
+        <v>187</v>
       </c>
       <c r="D26" s="4">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="E26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F26" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>7</v>
+        <v>190</v>
+      </c>
+      <c r="D27" s="4">
+        <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>8</v>
+        <v>191</v>
       </c>
       <c r="F27" t="s">
-        <v>9</v>
+        <v>192</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>10</v>
+        <v>193</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>11</v>
+        <v>194</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>12</v>
+        <v>195</v>
       </c>
       <c r="E28" t="s">
-        <v>13</v>
+        <v>122</v>
       </c>
       <c r="F28" t="s">
-        <v>14</v>
+        <v>196</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>15</v>
+        <v>197</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>17</v>
+        <v>271</v>
+      </c>
+      <c r="D29" s="4">
+        <v>0</v>
       </c>
       <c r="E29" t="s">
-        <v>18</v>
+        <v>122</v>
       </c>
       <c r="F29" t="s">
-        <v>19</v>
+        <v>198</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>20</v>
+        <v>199</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="E30" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="F30" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="E31" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="F31" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="E32" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E33" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33" t="s">
+        <v>24</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E34" t="s">
         <v>28</v>
       </c>
-      <c r="F32" t="s">
-        <v>33</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" ht="165" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33">
-        <v>99</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E33" t="s">
-        <v>8</v>
-      </c>
-      <c r="F33" t="s">
-        <v>36</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34">
-        <v>27</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E34" t="s">
-        <v>8</v>
-      </c>
       <c r="F34" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
@@ -2480,59 +2477,59 @@
         <v>1</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="E35" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="F35" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" ht="165" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36">
-        <v>2</v>
+        <v>99</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E36" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="F36" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="E37" t="s">
         <v>8</v>
       </c>
       <c r="F37" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
@@ -2540,59 +2537,59 @@
         <v>1</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="E38" t="s">
         <v>8</v>
       </c>
       <c r="F38" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="E39" t="s">
         <v>18</v>
       </c>
       <c r="F39" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="E40" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="F40" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
@@ -2600,159 +2597,159 @@
         <v>1</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="E41" t="s">
         <v>8</v>
       </c>
       <c r="F41" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>275</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="E42" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F42" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="E43" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="F43" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="E44" t="s">
-        <v>76</v>
+        <v>8</v>
       </c>
       <c r="F44" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="E45" t="s">
-        <v>80</v>
+        <v>23</v>
       </c>
       <c r="F45" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>108</v>
+        <v>70</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>109</v>
+        <v>71</v>
       </c>
       <c r="E46" t="s">
-        <v>110</v>
+        <v>8</v>
       </c>
       <c r="F46" t="s">
-        <v>111</v>
-      </c>
-      <c r="G46" s="3">
-        <v>78438357082</v>
+        <v>72</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B47">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>112</v>
+        <v>74</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>113</v>
+        <v>75</v>
       </c>
       <c r="E47" t="s">
-        <v>114</v>
+        <v>76</v>
       </c>
       <c r="F47" t="s">
-        <v>115</v>
+        <v>77</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>116</v>
+        <v>266</v>
       </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B48">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>117</v>
+        <v>78</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>118</v>
+        <v>79</v>
       </c>
       <c r="E48" t="s">
-        <v>119</v>
+        <v>80</v>
       </c>
       <c r="F48" t="s">
-        <v>120</v>
+        <v>81</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>121</v>
+        <v>82</v>
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.25">
@@ -2760,19 +2757,19 @@
         <v>1</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="E49" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="F49" t="s">
-        <v>86</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>87</v>
+        <v>111</v>
+      </c>
+      <c r="G49" s="3">
+        <v>78438357082</v>
       </c>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
@@ -2780,19 +2777,19 @@
         <v>1</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>215</v>
+        <v>112</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>216</v>
+        <v>113</v>
       </c>
       <c r="E50" t="s">
-        <v>217</v>
+        <v>114</v>
       </c>
       <c r="F50" t="s">
-        <v>218</v>
+        <v>115</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>219</v>
+        <v>116</v>
       </c>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.25">
@@ -2800,19 +2797,19 @@
         <v>1</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>220</v>
+        <v>117</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>221</v>
+        <v>118</v>
       </c>
       <c r="E51" t="s">
-        <v>222</v>
+        <v>119</v>
       </c>
       <c r="F51" t="s">
-        <v>223</v>
+        <v>120</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>221</v>
+        <v>121</v>
       </c>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.25">
@@ -2820,19 +2817,19 @@
         <v>1</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>224</v>
+        <v>83</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>225</v>
+        <v>84</v>
       </c>
       <c r="E52" t="s">
-        <v>226</v>
+        <v>85</v>
       </c>
       <c r="F52" t="s">
-        <v>227</v>
+        <v>86</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>225</v>
+        <v>87</v>
       </c>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.25">
@@ -2840,19 +2837,19 @@
         <v>1</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>228</v>
+        <v>205</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>229</v>
+        <v>206</v>
       </c>
       <c r="E53" t="s">
-        <v>230</v>
+        <v>207</v>
       </c>
       <c r="F53" t="s">
-        <v>231</v>
+        <v>208</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>232</v>
+        <v>209</v>
       </c>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
@@ -2860,19 +2857,19 @@
         <v>1</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>233</v>
+        <v>210</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>234</v>
+        <v>211</v>
       </c>
       <c r="E54" t="s">
-        <v>235</v>
+        <v>212</v>
       </c>
       <c r="F54" t="s">
-        <v>236</v>
+        <v>213</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>237</v>
+        <v>211</v>
       </c>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.25">
@@ -2880,39 +2877,39 @@
         <v>1</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>238</v>
+        <v>214</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>239</v>
+        <v>215</v>
       </c>
       <c r="E55" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
       <c r="F55" t="s">
-        <v>241</v>
+        <v>217</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>242</v>
+        <v>215</v>
       </c>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>243</v>
+        <v>218</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>244</v>
+        <v>219</v>
       </c>
       <c r="E56" t="s">
-        <v>245</v>
+        <v>220</v>
       </c>
       <c r="F56" t="s">
-        <v>246</v>
+        <v>221</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>247</v>
+        <v>222</v>
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.25">
@@ -2920,134 +2917,134 @@
         <v>1</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>248</v>
+        <v>223</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>249</v>
+        <v>224</v>
       </c>
       <c r="E57" t="s">
-        <v>250</v>
+        <v>225</v>
       </c>
       <c r="F57" t="s">
-        <v>251</v>
+        <v>226</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>252</v>
+        <v>227</v>
       </c>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B58">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>253</v>
+        <v>228</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>254</v>
+        <v>229</v>
       </c>
       <c r="E58" t="s">
-        <v>255</v>
+        <v>230</v>
       </c>
       <c r="F58" t="s">
-        <v>256</v>
+        <v>231</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>257</v>
+        <v>232</v>
       </c>
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B59">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>277</v>
+        <v>233</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>278</v>
+        <v>234</v>
       </c>
       <c r="E59" t="s">
-        <v>258</v>
-      </c>
-      <c r="J59" s="3"/>
+        <v>235</v>
+      </c>
+      <c r="F59" t="s">
+        <v>236</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="60" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B60">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>259</v>
+        <v>238</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>260</v>
+        <v>239</v>
       </c>
       <c r="E60" t="s">
-        <v>261</v>
+        <v>240</v>
       </c>
       <c r="F60" t="s">
-        <v>262</v>
+        <v>241</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>263</v>
+        <v>242</v>
       </c>
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B61">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>264</v>
+        <v>243</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>265</v>
+        <v>244</v>
       </c>
       <c r="E61" t="s">
-        <v>266</v>
+        <v>245</v>
       </c>
       <c r="F61" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>268</v>
+        <v>247</v>
       </c>
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B62">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E62" t="s">
-        <v>271</v>
-      </c>
-      <c r="F62" t="s">
-        <v>272</v>
-      </c>
-      <c r="G62" s="3" t="s">
-        <v>273</v>
-      </c>
+        <v>248</v>
+      </c>
+      <c r="J62" s="3"/>
     </row>
     <row r="63" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B63">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>210</v>
+        <v>249</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>211</v>
+        <v>250</v>
       </c>
       <c r="E63" t="s">
-        <v>212</v>
+        <v>251</v>
       </c>
       <c r="F63" t="s">
-        <v>213</v>
+        <v>252</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>214</v>
+        <v>253</v>
       </c>
     </row>
     <row r="64" spans="2:10" x14ac:dyDescent="0.25">
@@ -3055,19 +3052,19 @@
         <v>2</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>88</v>
+        <v>254</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>89</v>
+        <v>255</v>
       </c>
       <c r="E64" t="s">
-        <v>90</v>
+        <v>256</v>
       </c>
       <c r="F64" t="s">
-        <v>91</v>
+        <v>257</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>92</v>
+        <v>258</v>
       </c>
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.25">
@@ -3075,73 +3072,133 @@
         <v>1</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>93</v>
+        <v>259</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>279</v>
+        <v>260</v>
       </c>
       <c r="E65" t="s">
-        <v>94</v>
-      </c>
-      <c r="G65" s="3"/>
+        <v>261</v>
+      </c>
+      <c r="F65" t="s">
+        <v>262</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B66">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>95</v>
+        <v>200</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>96</v>
+        <v>201</v>
       </c>
       <c r="E66" t="s">
-        <v>97</v>
+        <v>202</v>
       </c>
       <c r="F66" t="s">
-        <v>98</v>
+        <v>203</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>99</v>
+        <v>204</v>
       </c>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B67">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>280</v>
+        <v>89</v>
       </c>
       <c r="E67" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="F67" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="E68" t="s">
+        <v>94</v>
+      </c>
+      <c r="G68" s="3"/>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B69">
+        <v>1</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E69" t="s">
+        <v>97</v>
+      </c>
+      <c r="F69" t="s">
+        <v>98</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="E70" t="s">
+        <v>101</v>
+      </c>
+      <c r="F70" t="s">
+        <v>102</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B71">
         <v>2</v>
       </c>
-      <c r="C68" s="5" t="s">
+      <c r="C71" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="D68" s="4" t="s">
+      <c r="D71" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E71" t="s">
         <v>106</v>
       </c>
-      <c r="F68" t="s">
+      <c r="F71" t="s">
         <v>107</v>
       </c>
-      <c r="G68" s="3">
+      <c r="G71" s="3">
         <v>470531000</v>
       </c>
     </row>
@@ -3167,7 +3224,7 @@
   <sheetData>
     <row r="1" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
@@ -3175,163 +3232,163 @@
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="2" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="C4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D4" t="s">
         <v>289</v>
       </c>
-      <c r="C4" t="s">
-        <v>305</v>
-      </c>
-      <c r="D4" t="s">
-        <v>299</v>
-      </c>
       <c r="E4" s="8" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="F4" s="8"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="6"/>
       <c r="C5" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="D5" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="C6" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="D6" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F6" s="8">
         <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="6"/>
       <c r="C7" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="D7" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="F7" s="8">
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="C8" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="D8" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="F8" s="8">
         <v>6</v>
       </c>
       <c r="G8" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
       <c r="C9" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="D9" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="F9" s="8">
         <v>4</v>
       </c>
       <c r="G9" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="C10" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="D10" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F10" s="8">
         <v>2</v>
       </c>
       <c r="G10" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="C11" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="D11" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="F11" s="8">
         <v>15</v>
       </c>
       <c r="G11" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>